<commit_message>
updated GA Solver excel
</commit_message>
<xml_diff>
--- a/workshop_01/SearchGA/ISBA03-SearchExercise GA Search v001.xlsx
+++ b/workshop_01/SearchGA/ISBA03-SearchExercise GA Search v001.xlsx
@@ -587,9 +587,9 @@
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="9" min="2" style="1" width="18.2105263157895"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="24.8502024291498"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="1" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="9" min="2" style="1" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="25.0647773279352"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="1" width="32.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -632,26 +632,26 @@
         <v>7</v>
       </c>
       <c r="C3" s="8" t="n">
-        <v>5000</v>
+        <v>100</v>
       </c>
       <c r="D3" s="9" t="n">
-        <v>12799.9979748306</v>
+        <v>200</v>
       </c>
       <c r="E3" s="9" t="n">
-        <v>2400</v>
+        <v>800</v>
       </c>
       <c r="F3" s="9" t="n">
-        <v>25599.9937680235</v>
+        <v>400</v>
       </c>
       <c r="G3" s="9" t="n">
-        <v>12799.9990751644</v>
+        <v>500</v>
       </c>
       <c r="H3" s="10" t="n">
-        <v>38399.9977915448</v>
+        <v>600</v>
       </c>
       <c r="I3" s="11" t="n">
         <f aca="false">SUM(C3:H3)</f>
-        <v>96999.9886095634</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -732,31 +732,31 @@
       </c>
       <c r="C7" s="24" t="n">
         <f aca="false">C$3*C4</f>
-        <v>1150</v>
+        <v>23</v>
       </c>
       <c r="D7" s="24" t="n">
         <f aca="false">D$3*D4</f>
-        <v>3839.99939244919</v>
+        <v>60</v>
       </c>
       <c r="E7" s="24" t="n">
         <f aca="false">E$3*E4</f>
-        <v>792</v>
+        <v>264</v>
       </c>
       <c r="F7" s="24" t="n">
         <f aca="false">F$3*F4</f>
-        <v>7679.99813040706</v>
+        <v>120</v>
       </c>
       <c r="G7" s="24" t="n">
         <f aca="false">G$3*G4</f>
-        <v>1791.99987052302</v>
+        <v>70</v>
       </c>
       <c r="H7" s="25" t="n">
         <f aca="false">H$3*H4</f>
-        <v>16511.9990503643</v>
+        <v>258</v>
       </c>
       <c r="I7" s="26" t="n">
         <f aca="false">SUM(C7:H7)</f>
-        <v>31765.9964437436</v>
+        <v>795</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -765,31 +765,31 @@
       </c>
       <c r="C8" s="27" t="n">
         <f aca="false">C$3*C5</f>
-        <v>210000</v>
+        <v>4200</v>
       </c>
       <c r="D8" s="27" t="n">
         <f aca="false">D$3*D5</f>
-        <v>511999.918993226</v>
+        <v>8000</v>
       </c>
       <c r="E8" s="27" t="n">
         <f aca="false">E$3*E5</f>
-        <v>108000</v>
+        <v>36000</v>
       </c>
       <c r="F8" s="27" t="n">
         <f aca="false">F$3*F5</f>
-        <v>1100799.73202501</v>
+        <v>17200</v>
       </c>
       <c r="G8" s="27" t="n">
         <f aca="false">G$3*G5</f>
-        <v>409599.970405262</v>
+        <v>16000</v>
       </c>
       <c r="H8" s="28" t="n">
         <f aca="false">H$3*H5</f>
-        <v>1958399.88736879</v>
+        <v>30600</v>
       </c>
       <c r="I8" s="29" t="n">
         <f aca="false">SUM(C8:H8)</f>
-        <v>4298799.50879229</v>
+        <v>112000</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -798,31 +798,31 @@
       </c>
       <c r="C9" s="27" t="n">
         <f aca="false">C$3*C6</f>
-        <v>75000</v>
+        <v>1500</v>
       </c>
       <c r="D9" s="27" t="n">
         <f aca="false">D$3*D6</f>
-        <v>268799.957471444</v>
+        <v>4200</v>
       </c>
       <c r="E9" s="27" t="n">
         <f aca="false">E$3*E6</f>
-        <v>55200</v>
+        <v>18400</v>
       </c>
       <c r="F9" s="27" t="n">
         <f aca="false">F$3*F6</f>
-        <v>614399.850432565</v>
+        <v>9600</v>
       </c>
       <c r="G9" s="27" t="n">
         <f aca="false">G$3*G6</f>
-        <v>166399.987977138</v>
+        <v>6500</v>
       </c>
       <c r="H9" s="28" t="n">
         <f aca="false">H$3*H6</f>
-        <v>1267199.92712098</v>
+        <v>19800</v>
       </c>
       <c r="I9" s="29" t="n">
         <f aca="false">SUM(C9:H9)</f>
-        <v>2446999.72300213</v>
+        <v>60000</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -831,31 +831,31 @@
       </c>
       <c r="C10" s="30" t="n">
         <f aca="false">C8-C9</f>
-        <v>135000</v>
+        <v>2700</v>
       </c>
       <c r="D10" s="30" t="n">
         <f aca="false">D8-D9</f>
-        <v>243199.961521782</v>
+        <v>3800</v>
       </c>
       <c r="E10" s="30" t="n">
         <f aca="false">E8-E9</f>
-        <v>52800</v>
+        <v>17600</v>
       </c>
       <c r="F10" s="30" t="n">
         <f aca="false">F8-F9</f>
-        <v>486399.881592447</v>
+        <v>7600</v>
       </c>
       <c r="G10" s="30" t="n">
         <f aca="false">G8-G9</f>
-        <v>243199.982428124</v>
+        <v>9500</v>
       </c>
       <c r="H10" s="31" t="n">
         <f aca="false">H8-H9</f>
-        <v>691199.960247807</v>
+        <v>10800</v>
       </c>
       <c r="I10" s="32" t="n">
         <f aca="false">SUM(C10:H10)</f>
-        <v>1851799.78579016</v>
+        <v>52000</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -869,7 +869,7 @@
     <row r="13" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="1" t="n">
         <f aca="false">D3/C3</f>
-        <v>2.55999959496613</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -883,7 +883,7 @@
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="1" t="n">
         <f aca="false">E3/G3</f>
-        <v>0.187500013547397</v>
+        <v>1.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>